<commit_message>
last changes to cost for midterm
</commit_message>
<xml_diff>
--- a/mass_input_cost_model.xlsx
+++ b/mass_input_cost_model.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>CONCEPT 1</t>
   </si>
@@ -28,19 +28,31 @@
     <t>CONCEPT 4</t>
   </si>
   <si>
+    <t>CONCEPT 5</t>
+  </si>
+  <si>
+    <t>CONCEPT 6</t>
+  </si>
+  <si>
     <t>DEV</t>
   </si>
   <si>
-    <t>Jarvis Hydrogen</t>
-  </si>
-  <si>
-    <t>Jarvis methane</t>
-  </si>
-  <si>
-    <t>Starship hydrogen</t>
-  </si>
-  <si>
-    <t>Starship methane</t>
+    <t>Lifting body - hydrolox</t>
+  </si>
+  <si>
+    <t>Lifting body - methalox</t>
+  </si>
+  <si>
+    <t>Blunt cone - hydrolox</t>
+  </si>
+  <si>
+    <t>Blunt cone - methalox</t>
+  </si>
+  <si>
+    <t>Starship - hydrolox</t>
+  </si>
+  <si>
+    <t>Starship - methalox</t>
   </si>
   <si>
     <t>Pressurizant Tank</t>
@@ -132,13 +144,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -149,7 +167,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -199,6 +217,13 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFc6c6c6"/>
       </left>
@@ -213,51 +238,56 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -564,549 +594,619 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="11" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="26.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="14.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="12" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="14" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="15" width="26.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="16" width="14.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="16" width="15.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="16" width="17.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="16" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="14" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="14" width="16.290714285714284" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>8</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1"/>
-      <c r="B3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="6">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6">
-        <v>0</v>
-      </c>
-      <c r="E3" s="6">
-        <v>0</v>
-      </c>
-      <c r="F3" s="6">
-        <v>0</v>
-      </c>
+      <c r="B3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1"/>
-      <c r="B4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="6">
+      <c r="B4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="7">
         <v>24406</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="7">
         <v>19362</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="9">
         <v>18355.92785</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="9">
         <v>12435.88633</v>
       </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1"/>
-      <c r="B5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="6">
+      <c r="B5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="7">
         <v>9258</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="7">
         <v>30285</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="9">
         <v>6953.632778</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="9">
         <v>18977.67058</v>
       </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1"/>
-      <c r="B6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="6">
-        <v>0</v>
-      </c>
-      <c r="D6" s="6">
-        <v>0</v>
-      </c>
-      <c r="E6" s="6">
-        <v>0</v>
-      </c>
-      <c r="F6" s="6">
-        <v>0</v>
-      </c>
+      <c r="B6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1"/>
-      <c r="B7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="6">
-        <v>0</v>
-      </c>
-      <c r="D7" s="6">
-        <v>0</v>
-      </c>
-      <c r="E7" s="6">
-        <v>0</v>
-      </c>
-      <c r="F7" s="6">
-        <v>0</v>
-      </c>
+      <c r="B7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1"/>
-      <c r="B8" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="6">
+      <c r="B8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="7">
         <v>600</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="7">
         <v>250</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="7">
         <v>600</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="7">
         <v>250</v>
       </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1"/>
-      <c r="B9" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="8">
+      <c r="B9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="9">
         <v>6540.980305</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="9">
         <v>13238.14295</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="9">
         <v>4113.568665</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="9">
         <v>8583.408099</v>
       </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1"/>
-      <c r="B10" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="8">
+      <c r="B10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="9">
         <v>1036.715299</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="9">
         <v>2104.075595</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="9">
         <v>649.8465685</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="9">
         <v>1362.227228</v>
       </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1"/>
-      <c r="B11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="6">
-        <v>0</v>
-      </c>
-      <c r="D11" s="6">
-        <v>0</v>
-      </c>
-      <c r="E11" s="6">
-        <v>0</v>
-      </c>
-      <c r="F11" s="6">
-        <v>0</v>
-      </c>
+      <c r="B11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0</v>
+      </c>
+      <c r="F11" s="7">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1"/>
-      <c r="B12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="6">
-        <v>0</v>
-      </c>
-      <c r="D12" s="6">
-        <v>0</v>
-      </c>
-      <c r="E12" s="6">
-        <v>0</v>
-      </c>
-      <c r="F12" s="6">
-        <v>0</v>
-      </c>
+      <c r="B12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0</v>
+      </c>
+      <c r="E12" s="7">
+        <v>0</v>
+      </c>
+      <c r="F12" s="7">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1"/>
-      <c r="B13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="6">
-        <v>0</v>
-      </c>
-      <c r="D13" s="6">
-        <v>0</v>
-      </c>
-      <c r="E13" s="6">
-        <v>0</v>
-      </c>
-      <c r="F13" s="6">
-        <v>0</v>
-      </c>
+      <c r="B13" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0</v>
+      </c>
+      <c r="E13" s="7">
+        <v>0</v>
+      </c>
+      <c r="F13" s="7">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1"/>
-      <c r="B14" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="6">
-        <v>0</v>
-      </c>
-      <c r="D14" s="6">
-        <v>0</v>
-      </c>
-      <c r="E14" s="6">
-        <v>0</v>
-      </c>
-      <c r="F14" s="6">
-        <v>0</v>
-      </c>
+      <c r="B14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0</v>
+      </c>
+      <c r="F14" s="7">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1"/>
-      <c r="B15" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="6">
-        <v>0</v>
-      </c>
-      <c r="D15" s="6">
-        <v>0</v>
-      </c>
-      <c r="E15" s="6">
-        <v>0</v>
-      </c>
-      <c r="F15" s="6">
-        <v>0</v>
-      </c>
+      <c r="B15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="7">
+        <v>0</v>
+      </c>
+      <c r="D15" s="7">
+        <v>0</v>
+      </c>
+      <c r="E15" s="7">
+        <v>0</v>
+      </c>
+      <c r="F15" s="7">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="1"/>
-      <c r="B16" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="8">
+      <c r="B16" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="9">
         <v>4996.547394</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="9">
         <v>3389.029716</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="9">
         <v>4104.236148</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="9">
         <v>2007.042678</v>
       </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="1"/>
-      <c r="B17" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="6">
-        <v>0</v>
-      </c>
-      <c r="D17" s="6">
-        <v>0</v>
-      </c>
-      <c r="E17" s="6">
-        <v>0</v>
-      </c>
-      <c r="F17" s="6">
-        <v>0</v>
-      </c>
+      <c r="B17" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="7">
+        <v>0</v>
+      </c>
+      <c r="D17" s="7">
+        <v>0</v>
+      </c>
+      <c r="E17" s="7">
+        <v>0</v>
+      </c>
+      <c r="F17" s="7">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="1"/>
-      <c r="B18" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="6">
+      <c r="B18" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="7">
         <v>719</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="7">
         <v>719</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="7">
         <v>719</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="7">
         <v>719</v>
       </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="1"/>
-      <c r="B19" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="6">
+      <c r="B19" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="7">
         <v>100</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="7">
         <v>100</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="7">
         <v>100</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="7">
         <v>100</v>
       </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="1"/>
-      <c r="B20" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="6">
+      <c r="B20" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="7">
         <v>100</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="7">
         <v>100</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="7">
         <v>100</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="7">
         <v>100</v>
       </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="1"/>
-      <c r="B21" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="8">
+      <c r="B21" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="9">
         <v>430.7601252</v>
       </c>
-      <c r="D21" s="8">
+      <c r="D21" s="9">
         <v>521.8894033</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21" s="9">
         <v>361.0996035</v>
       </c>
-      <c r="F21" s="8">
+      <c r="F21" s="9">
         <v>443.8290889</v>
       </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="1"/>
-      <c r="B22" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="8">
+      <c r="B22" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="9">
         <v>3.89364797</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D22" s="9">
         <v>4.161166159</v>
       </c>
-      <c r="E22" s="8">
+      <c r="E22" s="9">
         <v>3.662943339</v>
       </c>
-      <c r="F22" s="8">
+      <c r="F22" s="9">
         <v>3.934152917</v>
       </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="1"/>
-      <c r="B23" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="8">
+      <c r="B23" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="9">
         <v>525.1431317</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="9">
         <v>763.0925006</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="9">
         <v>1501.186006</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="9">
         <v>556.6151902</v>
       </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="1"/>
-      <c r="B24" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
+      <c r="B24" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="1"/>
-      <c r="B25" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25" s="8">
-        <v>296020.8381</v>
-      </c>
-      <c r="D25" s="8">
+      <c r="B25" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9">
+        <v>246684.0317</v>
+      </c>
+      <c r="F25" s="9">
         <v>600791.9647</v>
       </c>
-      <c r="E25" s="8">
+      <c r="G25" s="12">
         <v>185555.4038</v>
       </c>
-      <c r="F25" s="8">
+      <c r="H25" s="12">
         <v>388966.6202</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="1"/>
-      <c r="B26" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="8">
-        <v>262372.1506</v>
-      </c>
-      <c r="D26" s="8">
-        <v>543534.1034</v>
-      </c>
-      <c r="E26" s="8">
-        <v>164913.1903</v>
-      </c>
-      <c r="F26" s="8">
-        <v>352413.4919</v>
+      <c r="B26" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9">
+        <v>203643.4588</v>
+      </c>
+      <c r="F26" s="9">
+        <v>528534.1034</v>
+      </c>
+      <c r="G26" s="12">
+        <v>149913.1903</v>
+      </c>
+      <c r="H26" s="12">
+        <v>337413.4919</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="1"/>
-      <c r="B27" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27" s="6">
-        <v>0</v>
-      </c>
-      <c r="D27" s="6">
-        <v>0</v>
-      </c>
-      <c r="E27" s="6">
-        <v>0</v>
-      </c>
-      <c r="F27" s="6">
+      <c r="B27" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="7">
+        <v>0</v>
+      </c>
+      <c r="D27" s="7">
+        <v>0</v>
+      </c>
+      <c r="E27" s="7">
+        <v>0</v>
+      </c>
+      <c r="F27" s="7">
+        <v>0</v>
+      </c>
+      <c r="G27" s="13">
+        <v>0</v>
+      </c>
+      <c r="H27" s="13">
         <v>0</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="1"/>
-      <c r="B28" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C28" s="8">
-        <v>33648.68751</v>
-      </c>
-      <c r="D28" s="8">
-        <v>57257.86121</v>
-      </c>
-      <c r="E28" s="8">
-        <v>20642.21346</v>
-      </c>
-      <c r="F28" s="8">
-        <v>36553.12829</v>
+      <c r="B28" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9">
+        <v>43040.57</v>
+      </c>
+      <c r="F28" s="9">
+        <v>72257.86</v>
+      </c>
+      <c r="G28" s="12">
+        <v>35642.21</v>
+      </c>
+      <c r="H28" s="12">
+        <v>51553.13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
       <c r="A29" s="1"/>
-      <c r="B29" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C29" s="2">
+      <c r="B29" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="3">
         <v>6.03</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="3">
         <v>3.6</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="3">
         <v>6.03</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F29" s="3">
+        <v>3.6</v>
+      </c>
+      <c r="G29" s="12">
+        <v>6.03</v>
+      </c>
+      <c r="H29" s="12">
         <v>3.6</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="1"/>
-      <c r="B30" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="8">
-        <v>375.6802552</v>
-      </c>
-      <c r="D30" s="8">
-        <v>254.8142644</v>
-      </c>
-      <c r="E30" s="8">
-        <v>308.589184</v>
-      </c>
-      <c r="F30" s="8">
-        <v>150.9054645</v>
-      </c>
+      <c r="B30" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>